<commit_message>
add in day 3; stop tracking ~$ files; Add in "hawkN" oligo files; initialize library prep protocols;
Former-commit-id: bee9ca74d197cefbf4fd224bd510c891329fd956
</commit_message>
<xml_diff>
--- a/docs/20171205_lib2_ind/20171206.growth.xlsx
+++ b/docs/20171205_lib2_ind/20171206.growth.xlsx
@@ -421,7 +421,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B29" sqref="B29:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -904,21 +904,6 @@
       <c r="A29" t="s">
         <v>11</v>
       </c>
-      <c r="B29">
-        <v>145</v>
-      </c>
-      <c r="C29">
-        <f>B16</f>
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="D29">
-        <f>C16</f>
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="E29">
-        <f>D16</f>
-        <v>9.5000000000000001E-2</v>
-      </c>
       <c r="G29">
         <v>145</v>
       </c>
@@ -939,21 +924,6 @@
       <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="B30">
-        <v>235</v>
-      </c>
-      <c r="C30">
-        <f>10*B17</f>
-        <v>2.84</v>
-      </c>
-      <c r="D30">
-        <f>10*C17</f>
-        <v>2.7600000000000002</v>
-      </c>
-      <c r="E30">
-        <f>10*D17</f>
-        <v>2.9499999999999997</v>
-      </c>
       <c r="G30">
         <v>240</v>
       </c>
@@ -974,21 +944,6 @@
       <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="B31">
-        <v>290</v>
-      </c>
-      <c r="C31">
-        <f>10*6*B18</f>
-        <v>19.5</v>
-      </c>
-      <c r="D31">
-        <f>10*6*C18</f>
-        <v>18.18</v>
-      </c>
-      <c r="E31">
-        <f>10*6*D18</f>
-        <v>19.02</v>
-      </c>
       <c r="G31">
         <v>290</v>
       </c>
@@ -1008,21 +963,6 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
-      </c>
-      <c r="B32">
-        <v>340</v>
-      </c>
-      <c r="C32">
-        <f>10*6*6*B20</f>
-        <v>113.76</v>
-      </c>
-      <c r="D32">
-        <f>10*6*6*C20</f>
-        <v>110.88</v>
-      </c>
-      <c r="E32">
-        <f>10*6*6*D20</f>
-        <v>113.04</v>
       </c>
       <c r="G32">
         <v>337</v>

</xml_diff>